<commit_message>
Excel file template and first calculations programatically wrritten
</commit_message>
<xml_diff>
--- a/Report Pack/file.xlsx
+++ b/Report Pack/file.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="7160" yWindow="2900" windowWidth="22760" windowHeight="18480"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
@@ -14,22 +14,109 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>abc</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+  <si>
+    <t>Value of Approved Payments</t>
+  </si>
+  <si>
+    <t>Number of Declined/Approved</t>
+  </si>
+  <si>
+    <t>Average Surcharge Rate</t>
+  </si>
+  <si>
+    <t>Direct Debit Payments</t>
+  </si>
+  <si>
+    <t>Number of Approved Payments</t>
+  </si>
+  <si>
+    <t>Dishonored Direct Debits</t>
+  </si>
+  <si>
+    <t>Number of Active Authorities</t>
+  </si>
+  <si>
+    <t>Fee Finance</t>
+  </si>
+  <si>
+    <t>Fee Finance Loans</t>
+  </si>
+  <si>
+    <t>Fee Finance Quotes</t>
+  </si>
+  <si>
+    <t>Engagements</t>
+  </si>
+  <si>
+    <t>Engagements Sent</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Engagements by Status</t>
+  </si>
+  <si>
+    <t>Engagements Signed</t>
+  </si>
+  <si>
+    <t>Debtor Management</t>
+  </si>
+  <si>
+    <t>Aged Debt Trend</t>
+  </si>
+  <si>
+    <t>Number of Reminders Sent</t>
+  </si>
+  <si>
+    <t>Credit Insights</t>
+  </si>
+  <si>
+    <t>Credit Scores Descriptor</t>
+  </si>
+  <si>
+    <t>Clients Dropped Credit Status</t>
+  </si>
+  <si>
+    <t>Credit Scores by State</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="4"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <color rgb="4372c5"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="5"/>
+      <sz val="16"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -40,7 +127,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -48,12 +135,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -69,6 +172,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1179210</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -368,33 +520,376 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A5:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>235235</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5235</v>
-      </c>
-      <c r="B2">
+    <row r="5" ht="20" customHeight="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>44197</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44228</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44256</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44287</v>
+      </c>
+      <c r="F5" s="1">
+        <v>44317</v>
+      </c>
+      <c r="G5" s="1">
+        <v>44348</v>
+      </c>
+      <c r="H5" s="1">
+        <v>44378</v>
+      </c>
+    </row>
+    <row r="6" ht="22" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>40165.376000000004</v>
+      </c>
+      <c r="F6">
+        <v>83351.40400000001</v>
+      </c>
+      <c r="G6">
+        <v>77477.077</v>
+      </c>
+      <c r="H6">
+        <v>63772.048</v>
+      </c>
+      <c r="I6">
+        <v>78229.64300000001</v>
+      </c>
+      <c r="J6">
+        <v>81307.26049999999</v>
+      </c>
+      <c r="K6">
+        <v>37565.5125</v>
+      </c>
+      <c r="L6">
+        <v>99061.0655</v>
+      </c>
+    </row>
+    <row r="7" ht="19" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>40165.376000000004</v>
+      </c>
+      <c r="G7">
+        <v>83351.40400000001</v>
+      </c>
+      <c r="H7">
+        <v>77477.077</v>
+      </c>
+      <c r="I7">
+        <v>63772.048</v>
+      </c>
+      <c r="J7">
+        <v>78229.64300000001</v>
+      </c>
+      <c r="K7">
+        <v>81307.26049999999</v>
+      </c>
+      <c r="L7">
+        <v>37565.5125</v>
+      </c>
+      <c r="M7">
+        <v>99061.0655</v>
+      </c>
+    </row>
+    <row r="8" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
write for count of approved payments complete
</commit_message>
<xml_diff>
--- a/Report Pack/file.xlsx
+++ b/Report Pack/file.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+  <si>
+    <t>Count of Approved Payments</t>
+  </si>
   <si>
     <t>Value of Approved Payments</t>
   </si>
@@ -86,7 +89,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -104,6 +107,11 @@
     <font>
       <color rgb="4372c5"/>
       <sz val="14"/>
+    </font>
+    <font>
+      <color rgb="FF4372C5"/>
+      <sz val="14"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <color theme="1"/>
@@ -148,15 +156,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,13 +529,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:M28"/>
+  <dimension ref="A5:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="29.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
@@ -555,8 +564,8 @@
         <v>44378</v>
       </c>
     </row>
-    <row r="6" ht="22" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" ht="22" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B6">
@@ -569,33 +578,39 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>40165.376000000004</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>83351.40400000001</v>
+        <v>10</v>
       </c>
       <c r="G6">
-        <v>77477.077</v>
+        <v>15</v>
       </c>
       <c r="H6">
-        <v>63772.048</v>
+        <v>15</v>
       </c>
       <c r="I6">
-        <v>78229.64300000001</v>
+        <v>10</v>
       </c>
       <c r="J6">
-        <v>81307.26049999999</v>
+        <v>16</v>
       </c>
       <c r="K6">
-        <v>37565.5125</v>
+        <v>15</v>
       </c>
       <c r="L6">
-        <v>99061.0655</v>
+        <v>8</v>
+      </c>
+      <c r="M6">
+        <v>19</v>
+      </c>
+      <c r="N6">
+        <v>11</v>
       </c>
     </row>
     <row r="7" ht="19" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>0</v>
+      <c r="A7" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -635,258 +650,258 @@
       </c>
     </row>
     <row r="8" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="A13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="A15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="A16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="A17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
     </row>
     <row r="18" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="A18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="4" t="s">
+      <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="B19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="A20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="A21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="A22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="A23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="A24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
     </row>
     <row r="25" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="A25" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="A26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="A27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="A28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>